<commit_message>
Renamed TE ammo, balanced ammo stats for YP and TE
</commit_message>
<xml_diff>
--- a/Weapon and Ammo Stats.xlsx
+++ b/Weapon and Ammo Stats.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE657A47-DF29-46D4-980A-CFC2BD687130}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0910C46E-2D93-4F26-BD07-B67D55C89ABE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23085" yWindow="2850" windowWidth="11160" windowHeight="9495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Weapons" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="82">
   <si>
     <t>Name</t>
   </si>
@@ -221,25 +221,52 @@
     <t>Shred</t>
   </si>
   <si>
-    <t>TE Power Core</t>
-  </si>
-  <si>
-    <t>TE Power Charge</t>
-  </si>
-  <si>
-    <t>TE Concentrated Power Charge</t>
-  </si>
-  <si>
-    <t>TE Energy Canister</t>
-  </si>
-  <si>
     <t>Ammo</t>
   </si>
   <si>
     <t>Crush</t>
   </si>
   <si>
-    <t>K.I.</t>
+    <t>556x45mm NATO</t>
+  </si>
+  <si>
+    <t>Hybrid Ocelot</t>
+  </si>
+  <si>
+    <t>Hybrid Black Phanter Rifle</t>
+  </si>
+  <si>
+    <t>Kinetic impact</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Work</t>
+  </si>
+  <si>
+    <t>Speed</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>T55 Core</t>
+  </si>
+  <si>
+    <t>T76 Core</t>
+  </si>
+  <si>
+    <t>T90 Canister</t>
+  </si>
+  <si>
+    <t>T101 Core</t>
+  </si>
+  <si>
+    <t>Mass x 500</t>
+  </si>
+  <si>
+    <t>Bulk x 500</t>
   </si>
 </sst>
 </file>
@@ -275,7 +302,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -283,6 +310,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -566,7 +596,7 @@
   <dimension ref="A1:N50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -621,7 +651,7 @@
         <v>24</v>
       </c>
       <c r="N1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -1065,139 +1095,132 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="E12" s="1"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
+      <c r="A12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="C12" s="2">
+        <v>10</v>
+      </c>
+      <c r="D12">
+        <v>58</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>0.05</v>
+      </c>
+      <c r="G12">
+        <v>1.2</v>
+      </c>
+      <c r="H12">
+        <v>1.3</v>
+      </c>
+      <c r="I12" s="2">
+        <v>0.36</v>
+      </c>
+      <c r="J12">
+        <v>1.05</v>
+      </c>
+      <c r="K12">
+        <v>6</v>
+      </c>
+      <c r="L12" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="M12" s="3">
+        <v>35</v>
+      </c>
+      <c r="N12" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>69</v>
       </c>
       <c r="B13" s="2">
-        <v>5.75</v>
+        <v>1.35</v>
       </c>
       <c r="C13" s="2">
-        <v>4</v>
+        <v>2.4</v>
       </c>
       <c r="D13">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E13" s="1">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="F13">
-        <v>0.18</v>
+        <v>0.09</v>
       </c>
       <c r="G13">
-        <v>1.1499999999999999</v>
+        <v>0.7</v>
       </c>
       <c r="H13">
-        <v>2.2000000000000002</v>
+        <v>1.5</v>
       </c>
       <c r="I13" s="2">
-        <v>0.65</v>
+        <v>0.33</v>
       </c>
       <c r="J13">
-        <v>1.2</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="K13">
+        <v>3</v>
+      </c>
+      <c r="L13" s="3">
         <v>1</v>
       </c>
-      <c r="L13" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="M13" s="3">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="N13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="2">
-        <v>11</v>
-      </c>
-      <c r="C14" s="2">
-        <v>4</v>
-      </c>
-      <c r="D14">
-        <v>52</v>
-      </c>
-      <c r="E14" s="1">
-        <v>0.85</v>
-      </c>
-      <c r="F14">
-        <v>0.1</v>
-      </c>
-      <c r="G14">
-        <v>1.38</v>
-      </c>
-      <c r="H14">
-        <v>1.78</v>
-      </c>
-      <c r="I14" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="J14">
-        <v>1.4</v>
-      </c>
-      <c r="K14">
-        <v>5</v>
-      </c>
-      <c r="L14" s="3">
-        <v>4</v>
-      </c>
-      <c r="M14" s="3">
-        <v>25</v>
-      </c>
-      <c r="N14" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B15" s="2">
-        <v>8.1</v>
+        <v>5.75</v>
       </c>
       <c r="C15" s="2">
-        <v>12.5</v>
+        <v>4</v>
       </c>
       <c r="D15">
-        <v>78</v>
+        <v>12</v>
       </c>
       <c r="E15" s="1">
-        <v>0.95</v>
+        <v>0.6</v>
       </c>
       <c r="F15">
-        <v>0.1</v>
+        <v>0.18</v>
       </c>
       <c r="G15">
-        <v>1.78</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="H15">
-        <v>1.82</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I15" s="2">
-        <v>0.4</v>
+        <v>0.65</v>
       </c>
       <c r="J15">
-        <v>2.25</v>
+        <v>1.2</v>
       </c>
       <c r="K15">
-        <v>7</v>
-      </c>
-      <c r="L15" s="3">
-        <v>12</v>
+        <v>1</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="M15" s="3">
-        <v>80</v>
+        <v>8</v>
       </c>
       <c r="N15" t="s">
         <v>31</v>
@@ -1205,122 +1228,122 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B16" s="2">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C16" s="2">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D16">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="E16" s="1">
-        <v>1</v>
+        <v>0.85</v>
       </c>
       <c r="F16">
         <v>0.1</v>
       </c>
       <c r="G16">
-        <v>0.9</v>
+        <v>1.38</v>
       </c>
       <c r="H16">
-        <v>3.5</v>
+        <v>1.78</v>
       </c>
       <c r="I16" s="2">
-        <v>1.5</v>
+        <v>0.4</v>
       </c>
       <c r="J16">
-        <v>3.1</v>
+        <v>1.4</v>
       </c>
       <c r="K16">
-        <v>1</v>
-      </c>
-      <c r="L16" s="3" t="s">
-        <v>19</v>
+        <v>5</v>
+      </c>
+      <c r="L16" s="3">
+        <v>4</v>
       </c>
       <c r="M16" s="3">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="N16" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B17" s="2">
-        <v>4.3</v>
+        <v>8.1</v>
       </c>
       <c r="C17" s="2">
-        <v>11</v>
+        <v>12.5</v>
       </c>
       <c r="D17">
-        <v>18</v>
+        <v>78</v>
       </c>
       <c r="E17" s="1">
-        <v>0.65</v>
+        <v>0.95</v>
       </c>
       <c r="F17">
         <v>0.1</v>
       </c>
       <c r="G17">
-        <v>1.38</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>19</v>
+        <v>1.78</v>
+      </c>
+      <c r="H17">
+        <v>1.82</v>
       </c>
       <c r="I17" s="2">
         <v>0.4</v>
       </c>
       <c r="J17">
-        <v>2.5</v>
+        <v>2.25</v>
       </c>
       <c r="K17">
-        <v>1</v>
-      </c>
-      <c r="L17" s="3" t="s">
-        <v>19</v>
+        <v>7</v>
+      </c>
+      <c r="L17" s="3">
+        <v>12</v>
       </c>
       <c r="M17" s="3">
-        <v>6</v>
+        <v>80</v>
       </c>
       <c r="N17" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B18" s="2">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C18" s="2">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D18">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="E18" s="1">
-        <v>0.88</v>
+        <v>1</v>
       </c>
       <c r="F18">
         <v>0.1</v>
       </c>
       <c r="G18">
-        <v>0.88</v>
+        <v>0.9</v>
       </c>
       <c r="H18">
-        <v>4.5</v>
+        <v>3.5</v>
       </c>
       <c r="I18" s="2">
-        <v>4</v>
+        <v>1.5</v>
       </c>
       <c r="J18">
-        <v>3.8</v>
+        <v>3.1</v>
       </c>
       <c r="K18">
         <v>1</v>
@@ -1329,179 +1352,179 @@
         <v>19</v>
       </c>
       <c r="M18" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N18" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="E19" s="1"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
+      <c r="A19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="2">
+        <v>4.3</v>
+      </c>
+      <c r="C19" s="2">
+        <v>11</v>
+      </c>
+      <c r="D19">
+        <v>18</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0.65</v>
+      </c>
+      <c r="F19">
+        <v>0.1</v>
+      </c>
+      <c r="G19">
+        <v>1.38</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I19" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="J19">
+        <v>2.5</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M19" s="3">
+        <v>6</v>
+      </c>
+      <c r="N19" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B20" s="2">
-        <v>3.3</v>
+        <v>16</v>
       </c>
       <c r="C20" s="2">
-        <v>9.1999999999999993</v>
+        <v>12</v>
       </c>
       <c r="D20">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="E20" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="F20">
+        <v>0.1</v>
+      </c>
+      <c r="G20">
+        <v>0.88</v>
+      </c>
+      <c r="H20">
+        <v>4.5</v>
+      </c>
+      <c r="I20" s="2">
+        <v>4</v>
+      </c>
+      <c r="J20">
+        <v>3.8</v>
+      </c>
+      <c r="K20">
         <v>1</v>
       </c>
-      <c r="F20">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="G20">
-        <v>1.34</v>
-      </c>
-      <c r="H20">
-        <v>1.56</v>
-      </c>
-      <c r="I20" s="2">
-        <v>0.36</v>
-      </c>
-      <c r="J20">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="K20">
-        <v>5</v>
-      </c>
-      <c r="L20" s="3">
-        <v>6</v>
+      <c r="L20" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="M20" s="3">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="N20" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>41</v>
-      </c>
-      <c r="B21" s="2">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C21" s="2">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="D21">
-        <v>12</v>
-      </c>
-      <c r="E21" s="1">
-        <v>0.7</v>
-      </c>
-      <c r="F21">
-        <v>0.17</v>
-      </c>
-      <c r="G21">
-        <v>1.01</v>
-      </c>
-      <c r="H21">
-        <v>1.8</v>
-      </c>
-      <c r="I21" s="2">
-        <v>0.36</v>
-      </c>
-      <c r="J21">
-        <v>0.6</v>
-      </c>
-      <c r="K21">
-        <v>1</v>
-      </c>
-      <c r="L21" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="M21" s="3">
-        <v>12</v>
-      </c>
-      <c r="N21" t="s">
-        <v>67</v>
-      </c>
+      <c r="E21" s="1"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B22" s="2">
-        <v>4.5</v>
+        <v>3.3</v>
       </c>
       <c r="C22" s="2">
-        <v>12.1</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="D22">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="E22" s="1">
-        <v>2.6</v>
+        <v>1</v>
       </c>
       <c r="F22">
-        <v>0.08</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="G22">
-        <v>1.42</v>
+        <v>1.34</v>
       </c>
       <c r="H22">
-        <v>2.0099999999999998</v>
+        <v>1.56</v>
       </c>
       <c r="I22" s="2">
-        <v>0.5</v>
+        <v>0.36</v>
       </c>
       <c r="J22">
-        <v>1.3</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="K22">
-        <v>1</v>
-      </c>
-      <c r="L22" s="3" t="s">
-        <v>19</v>
+        <v>5</v>
+      </c>
+      <c r="L22" s="3">
+        <v>6</v>
       </c>
       <c r="M22" s="3">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="N22" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B23" s="2">
-        <v>4.1100000000000003</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="C23" s="2">
-        <v>10.6</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D23">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="E23" s="1">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="F23">
-        <v>0.21</v>
+        <v>0.17</v>
       </c>
       <c r="G23">
-        <v>1.38</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>19</v>
+        <v>1.01</v>
+      </c>
+      <c r="H23">
+        <v>1.8</v>
       </c>
       <c r="I23" s="2">
         <v>0.36</v>
       </c>
       <c r="J23">
-        <v>1.1000000000000001</v>
+        <v>0.6</v>
       </c>
       <c r="K23">
         <v>1</v>
@@ -1510,116 +1533,153 @@
         <v>19</v>
       </c>
       <c r="M23" s="3">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="N23" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B24" s="2">
-        <v>6.85</v>
+        <v>4.5</v>
       </c>
       <c r="C24" s="2">
-        <v>12.6</v>
+        <v>12.1</v>
       </c>
       <c r="D24">
         <v>75</v>
       </c>
       <c r="E24" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="F24">
+        <v>0.08</v>
+      </c>
+      <c r="G24">
+        <v>1.42</v>
+      </c>
+      <c r="H24">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="I24" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="J24">
+        <v>1.3</v>
+      </c>
+      <c r="K24">
         <v>1</v>
       </c>
-      <c r="F24">
-        <v>0.18</v>
-      </c>
-      <c r="G24">
-        <v>1.64</v>
-      </c>
-      <c r="H24">
-        <v>1.21</v>
-      </c>
-      <c r="I24" s="2">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="J24">
-        <v>1.25</v>
-      </c>
-      <c r="K24">
-        <v>3</v>
-      </c>
-      <c r="L24" s="3">
-        <v>12</v>
+      <c r="L24" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="M24" s="3">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="N24" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B25" s="2">
-        <v>10</v>
+        <v>4.1100000000000003</v>
       </c>
       <c r="C25" s="2">
-        <v>18</v>
+        <v>10.6</v>
       </c>
       <c r="D25">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="E25" s="1">
         <v>1</v>
       </c>
       <c r="F25">
-        <v>0.12</v>
+        <v>0.21</v>
       </c>
       <c r="G25">
-        <v>1.82</v>
-      </c>
-      <c r="H25">
-        <v>0.88</v>
+        <v>1.38</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="I25" s="2">
-        <v>2.6</v>
+        <v>0.36</v>
       </c>
       <c r="J25">
-        <v>3.8</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="K25">
-        <v>20</v>
-      </c>
-      <c r="L25" s="3">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="M25" s="3">
-        <v>200</v>
+        <v>10</v>
       </c>
       <c r="N25" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="E26" s="1"/>
-      <c r="L26" s="3"/>
-      <c r="M26" s="3"/>
+      <c r="A26" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="2">
+        <v>6.85</v>
+      </c>
+      <c r="C26" s="2">
+        <v>12.6</v>
+      </c>
+      <c r="D26">
+        <v>75</v>
+      </c>
+      <c r="E26" s="1">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>0.18</v>
+      </c>
+      <c r="G26">
+        <v>1.64</v>
+      </c>
+      <c r="H26">
+        <v>1.21</v>
+      </c>
+      <c r="I26" s="2">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="J26">
+        <v>1.25</v>
+      </c>
+      <c r="K26">
+        <v>3</v>
+      </c>
+      <c r="L26" s="3">
+        <v>12</v>
+      </c>
+      <c r="M26" s="3">
+        <v>30</v>
+      </c>
+      <c r="N26" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B27" s="2">
-        <v>3.12</v>
+        <v>10</v>
       </c>
       <c r="C27" s="2">
-        <v>8.1999999999999993</v>
+        <v>18</v>
       </c>
       <c r="D27">
         <v>55</v>
@@ -1628,290 +1688,331 @@
         <v>1</v>
       </c>
       <c r="F27">
-        <v>0.14000000000000001</v>
+        <v>0.12</v>
       </c>
       <c r="G27">
-        <v>1.21</v>
+        <v>1.82</v>
       </c>
       <c r="H27">
-        <v>1.48</v>
-      </c>
-      <c r="I27">
-        <v>0.36</v>
+        <v>0.88</v>
+      </c>
+      <c r="I27" s="2">
+        <v>2.6</v>
       </c>
       <c r="J27">
-        <v>0.6</v>
+        <v>3.8</v>
       </c>
       <c r="K27">
+        <v>20</v>
+      </c>
+      <c r="L27" s="3">
         <v>5</v>
       </c>
-      <c r="L27" s="3">
-        <v>3</v>
-      </c>
       <c r="M27" s="3">
-        <v>40</v>
+        <v>200</v>
       </c>
       <c r="N27" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>47</v>
-      </c>
-      <c r="B28" s="2">
-        <v>2.85</v>
-      </c>
-      <c r="C28" s="2">
-        <v>9.6999999999999993</v>
-      </c>
-      <c r="D28">
-        <v>32</v>
-      </c>
-      <c r="E28" s="1">
-        <v>1</v>
-      </c>
-      <c r="F28">
-        <v>0</v>
-      </c>
-      <c r="G28">
-        <v>0.91</v>
-      </c>
-      <c r="H28">
-        <v>1.37</v>
-      </c>
-      <c r="I28">
-        <v>0.36</v>
-      </c>
-      <c r="J28">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="K28">
-        <v>5</v>
-      </c>
-      <c r="L28" s="3">
-        <v>5</v>
-      </c>
-      <c r="M28" s="3">
-        <v>25</v>
-      </c>
-      <c r="N28" t="s">
-        <v>51</v>
-      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="E28" s="1"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B29" s="2">
-        <v>3.3</v>
+        <v>3.12</v>
       </c>
       <c r="C29" s="2">
-        <v>12.2</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="D29">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="E29" s="1">
-        <v>1.86</v>
+        <v>1</v>
       </c>
       <c r="F29">
-        <v>0.04</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="G29">
-        <v>1.52</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>19</v>
+        <v>1.21</v>
+      </c>
+      <c r="H29">
+        <v>1.48</v>
       </c>
       <c r="I29">
-        <v>0.5</v>
+        <v>0.36</v>
       </c>
       <c r="J29">
-        <v>1.3</v>
+        <v>0.6</v>
       </c>
       <c r="K29">
-        <v>1</v>
-      </c>
-      <c r="L29" s="3" t="s">
-        <v>19</v>
+        <v>5</v>
+      </c>
+      <c r="L29" s="3">
+        <v>3</v>
       </c>
       <c r="M29" s="3">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="N29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B30" s="2">
-        <v>2.3199999999999998</v>
+        <v>2.85</v>
       </c>
       <c r="C30" s="2">
-        <v>2.5</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="D30">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="E30" s="1">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="F30">
-        <v>0.12</v>
+        <v>0</v>
       </c>
       <c r="G30">
-        <v>1</v>
+        <v>0.91</v>
       </c>
       <c r="H30">
-        <v>1.74</v>
+        <v>1.37</v>
       </c>
       <c r="I30">
-        <v>0.38</v>
+        <v>0.36</v>
       </c>
       <c r="J30">
-        <v>0.6</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="K30">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="L30" s="3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M30" s="3">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="N30" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="C31" s="2">
+        <v>12.2</v>
+      </c>
+      <c r="D31">
+        <v>75</v>
+      </c>
+      <c r="E31" s="1">
+        <v>1.86</v>
+      </c>
+      <c r="F31">
+        <v>0.04</v>
+      </c>
+      <c r="G31">
+        <v>1.52</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I31">
+        <v>0.5</v>
+      </c>
+      <c r="J31">
+        <v>1.3</v>
+      </c>
+      <c r="K31">
+        <v>1</v>
+      </c>
+      <c r="L31" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M31" s="3">
+        <v>8</v>
+      </c>
+      <c r="N31" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32" s="2">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="C32" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="D32">
+        <v>12</v>
+      </c>
+      <c r="E32" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="F32">
+        <v>0.12</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32">
+        <v>1.74</v>
+      </c>
+      <c r="I32">
+        <v>0.38</v>
+      </c>
+      <c r="J32">
+        <v>0.6</v>
+      </c>
+      <c r="K32">
+        <v>2</v>
+      </c>
+      <c r="L32" s="3">
+        <v>0</v>
+      </c>
+      <c r="M32" s="3">
+        <v>12</v>
+      </c>
+      <c r="N32" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>50</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B33" s="2">
         <v>2.8</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C33" s="2">
         <v>4.8</v>
       </c>
-      <c r="D31">
+      <c r="D33">
         <v>14</v>
       </c>
-      <c r="E31" s="1">
+      <c r="E33" s="1">
         <v>1</v>
       </c>
-      <c r="F31">
+      <c r="F33">
         <v>0</v>
       </c>
-      <c r="G31">
+      <c r="G33">
         <v>0.89</v>
       </c>
-      <c r="H31">
+      <c r="H33">
         <v>1.24</v>
       </c>
-      <c r="I31">
+      <c r="I33">
         <v>0.36</v>
       </c>
-      <c r="J31">
+      <c r="J33">
         <v>0.6</v>
       </c>
-      <c r="K31">
+      <c r="K33">
         <v>5</v>
       </c>
-      <c r="L31" s="3">
+      <c r="L33" s="3">
         <v>3</v>
       </c>
-      <c r="M31" s="3">
+      <c r="M33" s="3">
         <v>30</v>
       </c>
-      <c r="N31" t="s">
+      <c r="N33" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="E32" s="1"/>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="E33" s="1"/>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="E34" s="1"/>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="E35" s="1"/>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="E36" s="1"/>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="E37" s="1"/>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="E38" s="1"/>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="E39" s="1"/>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="E40" s="1"/>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="E41" s="1"/>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="E42" s="1"/>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="E43" s="1"/>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="E44" s="1"/>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="E45" s="1"/>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="E46" s="1"/>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="E47" s="1"/>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="E48" s="1"/>
@@ -1934,10 +2035,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1161E47B-CE91-412B-8407-35405AE578FF}">
-  <dimension ref="A1:H182"/>
+  <dimension ref="A1:P182"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1945,11 +2046,12 @@
     <col min="1" max="1" width="28.28515625" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
     <col min="5" max="6" width="11.42578125" customWidth="1"/>
+    <col min="15" max="16" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1974,8 +2076,29 @@
       <c r="H1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" t="s">
+        <v>72</v>
+      </c>
+      <c r="M1" t="s">
+        <v>73</v>
+      </c>
+      <c r="O1" t="s">
+        <v>80</v>
+      </c>
+      <c r="P1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -2000,8 +2123,31 @@
       <c r="H2" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2">
+        <v>95</v>
+      </c>
+      <c r="J2">
+        <v>0.01</v>
+      </c>
+      <c r="K2">
+        <v>0.02</v>
+      </c>
+      <c r="L2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M2">
+        <v>1750</v>
+      </c>
+      <c r="O2">
+        <f>J2*500</f>
+        <v>5</v>
+      </c>
+      <c r="P2">
+        <f>K2*500</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -2026,8 +2172,31 @@
       <c r="H3" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <v>95</v>
+      </c>
+      <c r="J3">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="K3">
+        <v>0.01</v>
+      </c>
+      <c r="L3">
+        <v>0.03</v>
+      </c>
+      <c r="M3">
+        <v>1750</v>
+      </c>
+      <c r="O3">
+        <f t="shared" ref="O3:O16" si="0">J3*500</f>
+        <v>4.5</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P16" si="1">K3*500</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -2052,8 +2221,31 @@
       <c r="H4" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <v>78</v>
+      </c>
+      <c r="J4">
+        <v>0.02</v>
+      </c>
+      <c r="K4">
+        <v>0.02</v>
+      </c>
+      <c r="L4">
+        <v>0.06</v>
+      </c>
+      <c r="M4">
+        <v>2000</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -2078,8 +2270,31 @@
       <c r="H5" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5">
+        <v>231</v>
+      </c>
+      <c r="J5">
+        <v>1.2E-2</v>
+      </c>
+      <c r="K5">
+        <v>0.03</v>
+      </c>
+      <c r="L5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M5">
+        <v>2250</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -2104,13 +2319,36 @@
       <c r="H6" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <v>101</v>
+      </c>
+      <c r="J6">
+        <v>0.04</v>
+      </c>
+      <c r="K6">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L6">
+        <v>0.1</v>
+      </c>
+      <c r="M6" t="s">
+        <v>75</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>34</v>
       </c>
       <c r="B7" s="3">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="C7" s="3">
         <v>0.9</v>
@@ -2119,7 +2357,7 @@
         <v>57</v>
       </c>
       <c r="E7" s="3">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>61</v>
@@ -2130,8 +2368,31 @@
       <c r="H7" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7">
+        <v>120</v>
+      </c>
+      <c r="J7">
+        <v>0.04</v>
+      </c>
+      <c r="K7">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L7">
+        <v>0.1</v>
+      </c>
+      <c r="M7" t="s">
+        <v>75</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -2156,8 +2417,31 @@
       <c r="H8" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <v>101</v>
+      </c>
+      <c r="J8">
+        <v>0.04</v>
+      </c>
+      <c r="K8">
+        <v>0.09</v>
+      </c>
+      <c r="L8">
+        <v>0.1</v>
+      </c>
+      <c r="M8" t="s">
+        <v>75</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>59</v>
       </c>
@@ -2182,8 +2466,31 @@
       <c r="H9" s="3">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9">
+        <v>70</v>
+      </c>
+      <c r="J9">
+        <v>3.75</v>
+      </c>
+      <c r="K9">
+        <v>4.2</v>
+      </c>
+      <c r="L9">
+        <v>21.54</v>
+      </c>
+      <c r="M9" t="s">
+        <v>75</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="0"/>
+        <v>1875</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="1"/>
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>53</v>
       </c>
@@ -2208,8 +2515,31 @@
       <c r="H10" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10">
+        <v>101</v>
+      </c>
+      <c r="J10">
+        <v>1.2E-2</v>
+      </c>
+      <c r="K10">
+        <v>0.03</v>
+      </c>
+      <c r="L10">
+        <v>0.08</v>
+      </c>
+      <c r="M10">
+        <v>2000</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>51</v>
       </c>
@@ -2234,8 +2564,31 @@
       <c r="H11" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11">
+        <v>231</v>
+      </c>
+      <c r="J11">
+        <v>0.01</v>
+      </c>
+      <c r="K11">
+        <v>0.02</v>
+      </c>
+      <c r="L11">
+        <v>0.09</v>
+      </c>
+      <c r="M11">
+        <v>2750</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>52</v>
       </c>
@@ -2260,10 +2613,33 @@
       <c r="H12" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <v>201</v>
+      </c>
+      <c r="J12">
+        <v>0.02</v>
+      </c>
+      <c r="K12">
+        <v>0.05</v>
+      </c>
+      <c r="L12">
+        <v>0.16</v>
+      </c>
+      <c r="M12">
+        <v>3200</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="B13" s="3">
         <v>10</v>
@@ -2272,7 +2648,7 @@
         <v>0.4</v>
       </c>
       <c r="D13" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>19</v>
@@ -2286,10 +2662,33 @@
       <c r="H13" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13">
+        <v>160</v>
+      </c>
+      <c r="J13">
+        <v>0.03</v>
+      </c>
+      <c r="K13">
+        <v>0.02</v>
+      </c>
+      <c r="L13">
+        <v>0.12</v>
+      </c>
+      <c r="M13">
+        <v>3300</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="B14" s="3">
         <v>20</v>
@@ -2298,7 +2697,7 @@
         <v>0.4</v>
       </c>
       <c r="D14" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>19</v>
@@ -2312,10 +2711,33 @@
       <c r="H14" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <v>140</v>
+      </c>
+      <c r="J14">
+        <v>0.05</v>
+      </c>
+      <c r="K14">
+        <v>0.03</v>
+      </c>
+      <c r="L14">
+        <v>0.18</v>
+      </c>
+      <c r="M14">
+        <v>4500</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="B15" s="3">
         <v>20</v>
@@ -2324,7 +2746,7 @@
         <v>0.4</v>
       </c>
       <c r="D15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>19</v>
@@ -2338,10 +2760,33 @@
       <c r="H15" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15" s="5">
+        <v>70</v>
+      </c>
+      <c r="J15" s="5">
+        <v>0.06</v>
+      </c>
+      <c r="K15" s="5">
+        <v>0.04</v>
+      </c>
+      <c r="L15" s="5">
+        <v>0.62</v>
+      </c>
+      <c r="M15" s="5">
+        <v>5000</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="B16" s="3">
         <v>8</v>
@@ -2350,7 +2795,7 @@
         <v>0.4</v>
       </c>
       <c r="D16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>19</v>
@@ -2363,6 +2808,29 @@
       </c>
       <c r="H16" s="3" t="s">
         <v>19</v>
+      </c>
+      <c r="I16">
+        <v>300</v>
+      </c>
+      <c r="J16">
+        <v>0.03</v>
+      </c>
+      <c r="K16">
+        <v>0.02</v>
+      </c>
+      <c r="L16">
+        <v>0.36</v>
+      </c>
+      <c r="M16">
+        <v>7000</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="1"/>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update Weapon and Ammo Stats.xlsx
</commit_message>
<xml_diff>
--- a/Weapon and Ammo Stats.xlsx
+++ b/Weapon and Ammo Stats.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0910C46E-2D93-4F26-BD07-B67D55C89ABE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE38DE50-29F7-4F09-BF76-78E89242A60A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2910" yWindow="3735" windowWidth="19500" windowHeight="11715" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Weapons" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="84">
   <si>
     <t>Name</t>
   </si>
@@ -267,6 +267,12 @@
   </si>
   <si>
     <t>Bulk x 500</t>
+  </si>
+  <si>
+    <t>YP Microwave Gun</t>
+  </si>
+  <si>
+    <t>Microwave Bullet</t>
   </si>
 </sst>
 </file>
@@ -595,8 +601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N27" sqref="N27"/>
+    <sheetView topLeftCell="B17" workbookViewId="0">
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1943,9 +1949,48 @@
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="E34" s="1"/>
+      <c r="A34" t="s">
+        <v>82</v>
+      </c>
+      <c r="B34" s="2">
+        <v>4.32</v>
+      </c>
+      <c r="C34" s="2">
+        <v>11.6</v>
+      </c>
+      <c r="D34">
+        <v>32</v>
+      </c>
+      <c r="E34" s="1">
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <v>0.16</v>
+      </c>
+      <c r="G34">
+        <v>1.41</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I34">
+        <v>0.6</v>
+      </c>
+      <c r="J34">
+        <v>1.2</v>
+      </c>
+      <c r="K34">
+        <v>1</v>
+      </c>
+      <c r="L34" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M34" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N34" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B35" s="2"/>
@@ -2037,8 +2082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1161E47B-CE91-412B-8407-35405AE578FF}">
   <dimension ref="A1:P182"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2299,7 +2344,7 @@
         <v>31</v>
       </c>
       <c r="B6" s="3">
-        <v>9.5</v>
+        <v>9</v>
       </c>
       <c r="C6" s="3">
         <v>0.98</v>
@@ -2397,7 +2442,7 @@
         <v>39</v>
       </c>
       <c r="B8" s="3">
-        <v>8.1999999999999993</v>
+        <v>8</v>
       </c>
       <c r="C8" s="3">
         <v>0.98</v>

</xml_diff>